<commit_message>
cds SCRIPTS 1-10 obj correction input file correction
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC03_CDS_Filter_PHSAccession-phs001554.xlsx
+++ b/InputFiles/CDS/TC03_CDS_Filter_PHSAccession-phs001554.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation 0707\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\MarchBranch\Commons_Automation\InputFiles\CDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{5716A2CC-32C8-4991-82E0-0821F4E04FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31EECC3B-3639-4E31-AAFD-7C59C4EEB7EE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B133091-6F8E-4590-91DB-9C8A20A41114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -56,8 +56,14 @@
     <t>ParticipantsTab</t>
   </si>
   <si>
+    <t>SamplesTab</t>
+  </si>
+  <si>
+    <t>FilesTab</t>
+  </si>
+  <si>
     <t>WITH {
-    phs_accession: "phs001524",
+    phs_accession: "phs001554",
     subject_ids: [],
     experimental_strategies: [],
     genders: [],
@@ -144,7 +150,7 @@
   </si>
   <si>
     <t>WITH {
-    phs_accession: "phs001524",
+    phs_accession: "phs001554",
     subject_ids: [],
     experimental_strategies: [],
     genders: [],
@@ -307,17 +313,8 @@
     num_files AS `Files`</t>
   </si>
   <si>
-    <t>TC02_CDS_Filter_PHSAccession-phs001524_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC02_CDS_Filter_PHSAccession-phs001524_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>SamplesTab</t>
-  </si>
-  <si>
     <t>WITH {
-    phs_accession: "phs001524",
+    phs_accession: "phs001554",
     subject_ids: [],
     experimental_strategies: [],
     genders: [],
@@ -407,13 +404,16 @@
 LIMIT 100</t>
   </si>
   <si>
-    <t>FilesTab</t>
+    <t>TC03_CDS_Filter_PHSAccession-phs001554_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC03_CDS_Filter_PHSAccession-phs001554_WebData.xlsx</t>
   </si>
   <si>
     <t>WITH {
-    phs_accession: "phs001524",
+    phs_accession: "phs001554",
     subject_ids: [],
-    experimental_strategies: ["RNA-Seq"],
+    experimental_strategies: [],
     genders: [],
     sample_tumor_statuses: [],
     file_types: [],
@@ -506,7 +506,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,8 +568,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -890,10 +890,10 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="75.7109375" style="1" customWidth="1"/>
@@ -902,7 +902,7 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -919,62 +919,62 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.6">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="409.6">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="409.6">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
     </row>
@@ -1241,13 +1241,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B39B34C6-EFDB-4541-AABC-D7AE06D49FBB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B39B34C6-EFDB-4541-AABC-D7AE06D49FBB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f85370dd-8bed-4563-966d-78f0aeaadda0"/>
+    <ds:schemaRef ds:uri="fb9100ea-f450-491f-b913-6bafe2014090"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E99EBB6-1581-4825-93AF-8B3767B76F4C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E99EBB6-1581-4825-93AF-8B3767B76F4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EA3C331-1C22-47B8-86DA-5BAFBAC927CC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EA3C331-1C22-47B8-86DA-5BAFBAC927CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f85370dd-8bed-4563-966d-78f0aeaadda0"/>
+    <ds:schemaRef ds:uri="fb9100ea-f450-491f-b913-6bafe2014090"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>